<commit_message>
1. Added new test and updated an existing one.
</commit_message>
<xml_diff>
--- a/test/core/Test-Cases-Key.xlsx
+++ b/test/core/Test-Cases-Key.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="75">
   <si>
     <t>Test Name</t>
   </si>
@@ -233,6 +233,12 @@
   </si>
   <si>
     <t>Input files with file and gsiftp URL's</t>
+  </si>
+  <si>
+    <t>T10D</t>
+  </si>
+  <si>
+    <t>010-runtime-clustering - runtime-sharedfs-all-staging-nogridstart</t>
   </si>
 </sst>
 </file>
@@ -290,9 +296,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -310,6 +313,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -612,42 +618,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="A5" sqref="A5:K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="4" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="10" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="40" style="9" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="60.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40" style="8" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -662,10 +668,10 @@
       <c r="D2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="1" t="s">
         <v>34</v>
       </c>
@@ -678,7 +684,7 @@
       <c r="J2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>40</v>
       </c>
     </row>
@@ -702,370 +708,396 @@
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="6" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="K14" s="8" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K15" s="7" t="s">
+      <c r="K15" s="6" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K16" s="7" t="s">
+      <c r="E16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K16" s="6" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K17" s="7" t="s">
+      <c r="E17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K17" s="6" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="E22" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="I23" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="J23" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I23" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J23" s="4" t="s">
+      <c r="I24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J24" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I24" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J24" s="4" t="s">
+      <c r="I25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J25" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E26" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I25" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J25" s="4" t="s">
+      <c r="I26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J26" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E27" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="H27" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J27" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H26" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J26" s="4" t="s">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="J28" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J27" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="J28" s="4" t="s">
+      <c r="E29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J29" s="3" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating key for newly added test case.
</commit_message>
<xml_diff>
--- a/test/core/Test-Cases-Key.xlsx
+++ b/test/core/Test-Cases-Key.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="24795" windowHeight="11460"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="82">
   <si>
     <t>Test Name</t>
   </si>
@@ -239,6 +239,27 @@
   </si>
   <si>
     <t>010-runtime-clustering - runtime-sharedfs-all-staging-nogridstart</t>
+  </si>
+  <si>
+    <t>T15</t>
+  </si>
+  <si>
+    <t>Hierarchic workflow test.</t>
+  </si>
+  <si>
+    <t>015-shell-hierarchic-workflow</t>
+  </si>
+  <si>
+    <t>014-planner-performance</t>
+  </si>
+  <si>
+    <t>013-pegasus-mpi-cluster</t>
+  </si>
+  <si>
+    <t>T014</t>
+  </si>
+  <si>
+    <t>TESTMPIDAG</t>
   </si>
 </sst>
 </file>
@@ -618,16 +639,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:K29"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="60.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="3" customWidth="1"/>
@@ -1101,6 +1122,36 @@
         <v>37</v>
       </c>
     </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K32" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="E2:F2"/>

</xml_diff>